<commit_message>
updated stimuli for testing
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_ED/Trials/StimuliNegative_1.xlsx
+++ b/01_Paradigms/ER-ED/ER_ED/Trials/StimuliNegative_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_COG-ER-ED\COG-ER-ED\01_Paradigms\ER-ED\ER_ED\Stimuli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_CERED\CAD\01_Paradigms\ER-ED\ER_ED\Trials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17376" windowHeight="4872"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="4875"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="8">
   <si>
     <t>ImageFile</t>
   </si>
@@ -45,61 +45,10 @@
     <t>Stimuli/255.jpg</t>
   </si>
   <si>
-    <t>Stimuli/327.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9920.jpg</t>
-  </si>
-  <si>
     <t>Stimuli/225.jpg</t>
   </si>
   <si>
     <t>Stimuli/230.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/1111.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/3017.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/3022.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/3180.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/3280.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/6190.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/6244.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/6836.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9180.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9182.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9253.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9300.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9326.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9424.jpg</t>
-  </si>
-  <si>
-    <t>Stimuli/9425.jpg</t>
   </si>
 </sst>
 </file>
@@ -419,117 +368,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="A5" sqref="A5:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -545,9 +409,9 @@
       <selection activeCell="E2" sqref="E2:E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -562,7 +426,7 @@
         <v>Stimuli/234.jpg</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -577,7 +441,7 @@
         <v>Stimuli/248.jpg</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -592,7 +456,7 @@
         <v>Stimuli/3068.jpg</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,7 +471,7 @@
         <v>Stimuli/3069.jpg</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -622,7 +486,7 @@
         <v>Stimuli/3181.jpg</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -637,7 +501,7 @@
         <v>Stimuli/3225.jpg</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -652,7 +516,7 @@
         <v>Stimuli/3266.jpg</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -667,7 +531,7 @@
         <v>Stimuli/3400.jpg</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,7 +546,7 @@
         <v>Stimuli/3550.jpg</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -697,7 +561,7 @@
         <v>Stimuli/6350.jpg</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,7 +576,7 @@
         <v>Stimuli/6520.jpg</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -727,7 +591,7 @@
         <v>Stimuli/8485.jpg</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -742,7 +606,7 @@
         <v>Stimuli/9040.jpg</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -757,7 +621,7 @@
         <v>Stimuli/9140.jpg</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -772,7 +636,7 @@
         <v>Stimuli/9163.jpg</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
@@ -787,7 +651,7 @@
         <v>Stimuli/9181.jpg</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
@@ -802,7 +666,7 @@
         <v>Stimuli/9182.jpg</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
@@ -817,7 +681,7 @@
         <v>Stimuli/9183.jpg</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,7 +696,7 @@
         <v>Stimuli/9325.jpg</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
@@ -847,7 +711,7 @@
         <v>Stimuli/9414.jpg</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
@@ -862,7 +726,7 @@
         <v>Stimuli/9419.jpg</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
@@ -877,7 +741,7 @@
         <v>Stimuli/9424.jpg</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
@@ -892,7 +756,7 @@
         <v>Stimuli/9480.jpg</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -907,7 +771,7 @@
         <v>Stimuli/9635.1.jpg</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
@@ -922,7 +786,7 @@
         <v>Stimuli/9904.jpg</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
@@ -937,7 +801,7 @@
         <v>Stimuli/237.jpg</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
@@ -952,7 +816,7 @@
         <v>Stimuli/239.jpg</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
@@ -967,7 +831,7 @@
         <v>Stimuli/240.jpg</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
@@ -982,7 +846,7 @@
         <v>Stimuli/247.jpg</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
@@ -997,7 +861,7 @@
         <v>Stimuli/1111.jpg</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1012,7 +876,7 @@
         <v>Stimuli/1280.jpg</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +891,7 @@
         <v>Stimuli/3000.jpg</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +906,7 @@
         <v>Stimuli/3015.jpg</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +921,7 @@
         <v>Stimuli/3030.jpg</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1072,7 +936,7 @@
         <v>Stimuli/3051.jpg</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +951,7 @@
         <v>Stimuli/3063.jpg</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +966,7 @@
         <v>Stimuli/3150.jpg</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>3</v>
       </c>
@@ -1117,7 +981,7 @@
         <v>Stimuli/3180.jpg</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +996,7 @@
         <v>Stimuli/3301.jpg</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1147,7 +1011,7 @@
         <v>Stimuli/6313.jpg</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1162,7 +1026,7 @@
         <v>Stimuli/6550.jpg</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1041,7 @@
         <v>Stimuli/7361.jpg</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
@@ -1192,7 +1056,7 @@
         <v>Stimuli/9300.jpg</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1207,7 +1071,7 @@
         <v>Stimuli/9332.jpg</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1222,7 +1086,7 @@
         <v>Stimuli/9400.jpg</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1237,7 +1101,7 @@
         <v>Stimuli/9412.jpg</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1252,7 +1116,7 @@
         <v>Stimuli/9413.jpg</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1267,7 +1131,7 @@
         <v>Stimuli/9530.jpg</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1146,7 @@
         <v>Stimuli/9570.jpg</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1297,7 +1161,7 @@
         <v>Stimuli/9902.jpg</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1176,7 @@
         <v>Stimuli/242.jpg</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>3</v>
       </c>
@@ -1327,7 +1191,7 @@
         <v>Stimuli/252.jpg</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>3</v>
       </c>
@@ -1342,7 +1206,7 @@
         <v>Stimuli/3001.jpg</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>3</v>
       </c>
@@ -1357,7 +1221,7 @@
         <v>Stimuli/3010.jpg</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>3</v>
       </c>
@@ -1372,7 +1236,7 @@
         <v>Stimuli/3060.jpg</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
         <v>3</v>
       </c>
@@ -1387,7 +1251,7 @@
         <v>Stimuli/3071.jpg</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
@@ -1402,7 +1266,7 @@
         <v>Stimuli/3102.jpg</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>3</v>
       </c>
@@ -1417,7 +1281,7 @@
         <v>Stimuli/3140.jpg</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>3</v>
       </c>
@@ -1432,7 +1296,7 @@
         <v>Stimuli/6022.jpg</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>3</v>
       </c>
@@ -1447,7 +1311,7 @@
         <v>Stimuli/6831.jpg</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1326,7 @@
         <v>Stimuli/8230.jpg</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>3</v>
       </c>
@@ -1477,7 +1341,7 @@
         <v>Stimuli/8231.jpg</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1356,7 @@
         <v>Stimuli/9320.jpg</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
@@ -1507,7 +1371,7 @@
         <v>Stimuli/9410.jpg</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
@@ -1522,7 +1386,7 @@
         <v>Stimuli/9420.jpg</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>3</v>
       </c>
@@ -1537,7 +1401,7 @@
         <v>Stimuli/9423.jpg</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>3</v>
       </c>
@@ -1552,7 +1416,7 @@
         <v>Stimuli/9427.jpg</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1431,7 @@
         <v>Stimuli/9428.jpg</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1446,7 @@
         <v>Stimuli/9430.jpg</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>3</v>
       </c>
@@ -1597,7 +1461,7 @@
         <v>Stimuli/9500.jpg</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
         <v>3</v>
       </c>
@@ -1612,7 +1476,7 @@
         <v>Stimuli/9571.jpg</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1491,7 @@
         <v>Stimuli/9800.jpg</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>3</v>
       </c>
@@ -1642,7 +1506,7 @@
         <v>Stimuli/9908.jpg</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>3</v>
       </c>
@@ -1657,7 +1521,7 @@
         <v>Stimuli/9910.jpg</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>3</v>
       </c>
@@ -1672,7 +1536,7 @@
         <v>Stimuli/9940.jpg</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>3</v>
       </c>
@@ -1687,7 +1551,7 @@
         <v>Stimuli/233.jpg</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1566,7 @@
         <v>Stimuli/236.jpg</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>3</v>
       </c>
@@ -1717,7 +1581,7 @@
         <v>Stimuli/250.jpg</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>3</v>
       </c>
@@ -1732,7 +1596,7 @@
         <v>Stimuli/1300.jpg</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>3</v>
       </c>
@@ -1747,7 +1611,7 @@
         <v>Stimuli/3005.1.jpg</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>3</v>
       </c>
@@ -1762,7 +1626,7 @@
         <v>Stimuli/3053.jpg</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>3</v>
       </c>
@@ -1777,7 +1641,7 @@
         <v>Stimuli/3080.jpg</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
         <v>3</v>
       </c>
@@ -1792,7 +1656,7 @@
         <v>Stimuli/3168.jpg</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
         <v>3</v>
       </c>
@@ -1807,7 +1671,7 @@
         <v>Stimuli/3170.jpg</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +1686,7 @@
         <v>Stimuli/3350.jpg</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +1701,7 @@
         <v>Stimuli/3530.jpg</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
         <v>3</v>
       </c>
@@ -1852,7 +1716,7 @@
         <v>Stimuli/6212.jpg</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +1731,7 @@
         <v>Stimuli/6415.jpg</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
         <v>3</v>
       </c>
@@ -1882,7 +1746,7 @@
         <v>Stimuli/9250.jpg</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1" t="s">
         <v>3</v>
       </c>
@@ -1897,7 +1761,7 @@
         <v>Stimuli/9253.jpg</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
         <v>3</v>
       </c>
@@ -1912,7 +1776,7 @@
         <v>Stimuli/9373.jpg</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
@@ -1927,7 +1791,7 @@
         <v>Stimuli/9405.jpg</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>3</v>
       </c>
@@ -1942,7 +1806,7 @@
         <v>Stimuli/9421.jpg</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1" t="s">
         <v>3</v>
       </c>
@@ -1957,7 +1821,7 @@
         <v>Stimuli/9425.jpg</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
         <v>3</v>
       </c>
@@ -1972,7 +1836,7 @@
         <v>Stimuli/9433.jpg</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
         <v>3</v>
       </c>
@@ -1987,7 +1851,7 @@
         <v>Stimuli/9490.jpg</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
         <v>3</v>
       </c>
@@ -2002,7 +1866,7 @@
         <v>Stimuli/9520.jpg</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
         <v>3</v>
       </c>
@@ -2017,7 +1881,7 @@
         <v>Stimuli/9560.jpg</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
         <v>3</v>
       </c>
@@ -2032,7 +1896,7 @@
         <v>Stimuli/9599.jpg</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
deleted pics and added readme
</commit_message>
<xml_diff>
--- a/01_Paradigms/ER-ED/ER_ED/Trials/StimuliNegative_1.xlsx
+++ b/01_Paradigms/ER-ED/ER_ED/Trials/StimuliNegative_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_CERED\CAD\01_Paradigms\ER-ED\ER_ED\Trials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scheffel\Scheffel\Forschung\A_Projects\2021_COG-ER-ED\COG-ER-ED\01_Paradigms\ER-ED\ER_ED\Stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="4875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17376" windowHeight="4872"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="25">
   <si>
     <t>ImageFile</t>
   </si>
@@ -45,10 +45,61 @@
     <t>Stimuli/255.jpg</t>
   </si>
   <si>
+    <t>Stimuli/327.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9920.jpg</t>
+  </si>
+  <si>
     <t>Stimuli/225.jpg</t>
   </si>
   <si>
     <t>Stimuli/230.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/1111.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/3017.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/3022.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/3180.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/3280.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/6190.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/6244.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/6836.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9180.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9182.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9253.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9300.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9326.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9424.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/9425.jpg</t>
   </si>
 </sst>
 </file>
@@ -368,32 +419,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD19"/>
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -409,9 +545,9 @@
       <selection activeCell="E2" sqref="E2:E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -426,7 +562,7 @@
         <v>Stimuli/234.jpg</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -441,7 +577,7 @@
         <v>Stimuli/248.jpg</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -456,7 +592,7 @@
         <v>Stimuli/3068.jpg</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -471,7 +607,7 @@
         <v>Stimuli/3069.jpg</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -486,7 +622,7 @@
         <v>Stimuli/3181.jpg</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -501,7 +637,7 @@
         <v>Stimuli/3225.jpg</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -516,7 +652,7 @@
         <v>Stimuli/3266.jpg</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
@@ -531,7 +667,7 @@
         <v>Stimuli/3400.jpg</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -546,7 +682,7 @@
         <v>Stimuli/3550.jpg</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
@@ -561,7 +697,7 @@
         <v>Stimuli/6350.jpg</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -576,7 +712,7 @@
         <v>Stimuli/6520.jpg</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -591,7 +727,7 @@
         <v>Stimuli/8485.jpg</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
@@ -606,7 +742,7 @@
         <v>Stimuli/9040.jpg</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -621,7 +757,7 @@
         <v>Stimuli/9140.jpg</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
@@ -636,7 +772,7 @@
         <v>Stimuli/9163.jpg</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
@@ -651,7 +787,7 @@
         <v>Stimuli/9181.jpg</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
@@ -666,7 +802,7 @@
         <v>Stimuli/9182.jpg</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
@@ -681,7 +817,7 @@
         <v>Stimuli/9183.jpg</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
@@ -696,7 +832,7 @@
         <v>Stimuli/9325.jpg</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
@@ -711,7 +847,7 @@
         <v>Stimuli/9414.jpg</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
@@ -726,7 +862,7 @@
         <v>Stimuli/9419.jpg</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>3</v>
       </c>
@@ -741,7 +877,7 @@
         <v>Stimuli/9424.jpg</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
@@ -756,7 +892,7 @@
         <v>Stimuli/9480.jpg</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
@@ -771,7 +907,7 @@
         <v>Stimuli/9635.1.jpg</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
@@ -786,7 +922,7 @@
         <v>Stimuli/9904.jpg</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
@@ -801,7 +937,7 @@
         <v>Stimuli/237.jpg</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
@@ -816,7 +952,7 @@
         <v>Stimuli/239.jpg</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
@@ -831,7 +967,7 @@
         <v>Stimuli/240.jpg</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
@@ -846,7 +982,7 @@
         <v>Stimuli/247.jpg</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
@@ -861,7 +997,7 @@
         <v>Stimuli/1111.jpg</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
@@ -876,7 +1012,7 @@
         <v>Stimuli/1280.jpg</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
@@ -891,7 +1027,7 @@
         <v>Stimuli/3000.jpg</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
@@ -906,7 +1042,7 @@
         <v>Stimuli/3015.jpg</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
@@ -921,7 +1057,7 @@
         <v>Stimuli/3030.jpg</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
@@ -936,7 +1072,7 @@
         <v>Stimuli/3051.jpg</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
@@ -951,7 +1087,7 @@
         <v>Stimuli/3063.jpg</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
@@ -966,7 +1102,7 @@
         <v>Stimuli/3150.jpg</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>3</v>
       </c>
@@ -981,7 +1117,7 @@
         <v>Stimuli/3180.jpg</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
@@ -996,7 +1132,7 @@
         <v>Stimuli/3301.jpg</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +1147,7 @@
         <v>Stimuli/6313.jpg</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
@@ -1026,7 +1162,7 @@
         <v>Stimuli/6550.jpg</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1041,7 +1177,7 @@
         <v>Stimuli/7361.jpg</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1192,7 @@
         <v>Stimuli/9300.jpg</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1071,7 +1207,7 @@
         <v>Stimuli/9332.jpg</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
@@ -1086,7 +1222,7 @@
         <v>Stimuli/9400.jpg</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1101,7 +1237,7 @@
         <v>Stimuli/9412.jpg</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1116,7 +1252,7 @@
         <v>Stimuli/9413.jpg</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>3</v>
       </c>
@@ -1131,7 +1267,7 @@
         <v>Stimuli/9530.jpg</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1282,7 @@
         <v>Stimuli/9570.jpg</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1297,7 @@
         <v>Stimuli/9902.jpg</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>3</v>
       </c>
@@ -1176,7 +1312,7 @@
         <v>Stimuli/242.jpg</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
         <v>3</v>
       </c>
@@ -1191,7 +1327,7 @@
         <v>Stimuli/252.jpg</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
         <v>3</v>
       </c>
@@ -1206,7 +1342,7 @@
         <v>Stimuli/3001.jpg</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +1357,7 @@
         <v>Stimuli/3010.jpg</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="1" t="s">
         <v>3</v>
       </c>
@@ -1236,7 +1372,7 @@
         <v>Stimuli/3060.jpg</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>3</v>
       </c>
@@ -1251,7 +1387,7 @@
         <v>Stimuli/3071.jpg</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
@@ -1266,7 +1402,7 @@
         <v>Stimuli/3102.jpg</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>3</v>
       </c>
@@ -1281,7 +1417,7 @@
         <v>Stimuli/3140.jpg</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1432,7 @@
         <v>Stimuli/6022.jpg</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>3</v>
       </c>
@@ -1311,7 +1447,7 @@
         <v>Stimuli/6831.jpg</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1462,7 @@
         <v>Stimuli/8230.jpg</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="1" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1477,7 @@
         <v>Stimuli/8231.jpg</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
         <v>3</v>
       </c>
@@ -1356,7 +1492,7 @@
         <v>Stimuli/9320.jpg</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1507,7 @@
         <v>Stimuli/9410.jpg</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
@@ -1386,7 +1522,7 @@
         <v>Stimuli/9420.jpg</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
         <v>3</v>
       </c>
@@ -1401,7 +1537,7 @@
         <v>Stimuli/9423.jpg</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="1" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1552,7 @@
         <v>Stimuli/9427.jpg</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="1" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1567,7 @@
         <v>Stimuli/9428.jpg</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="1" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1582,7 @@
         <v>Stimuli/9430.jpg</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="1" t="s">
         <v>3</v>
       </c>
@@ -1461,7 +1597,7 @@
         <v>Stimuli/9500.jpg</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="1" t="s">
         <v>3</v>
       </c>
@@ -1476,7 +1612,7 @@
         <v>Stimuli/9571.jpg</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="1" t="s">
         <v>3</v>
       </c>
@@ -1491,7 +1627,7 @@
         <v>Stimuli/9800.jpg</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="1" t="s">
         <v>3</v>
       </c>
@@ -1506,7 +1642,7 @@
         <v>Stimuli/9908.jpg</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="1" t="s">
         <v>3</v>
       </c>
@@ -1521,7 +1657,7 @@
         <v>Stimuli/9910.jpg</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="1" t="s">
         <v>3</v>
       </c>
@@ -1536,7 +1672,7 @@
         <v>Stimuli/9940.jpg</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="1" t="s">
         <v>3</v>
       </c>
@@ -1551,7 +1687,7 @@
         <v>Stimuli/233.jpg</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="1" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1702,7 @@
         <v>Stimuli/236.jpg</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="1" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1717,7 @@
         <v>Stimuli/250.jpg</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>3</v>
       </c>
@@ -1596,7 +1732,7 @@
         <v>Stimuli/1300.jpg</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
         <v>3</v>
       </c>
@@ -1611,7 +1747,7 @@
         <v>Stimuli/3005.1.jpg</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
         <v>3</v>
       </c>
@@ -1626,7 +1762,7 @@
         <v>Stimuli/3053.jpg</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="1" t="s">
         <v>3</v>
       </c>
@@ -1641,7 +1777,7 @@
         <v>Stimuli/3080.jpg</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="1" t="s">
         <v>3</v>
       </c>
@@ -1656,7 +1792,7 @@
         <v>Stimuli/3168.jpg</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="1" t="s">
         <v>3</v>
       </c>
@@ -1671,7 +1807,7 @@
         <v>Stimuli/3170.jpg</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
         <v>3</v>
       </c>
@@ -1686,7 +1822,7 @@
         <v>Stimuli/3350.jpg</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="1" t="s">
         <v>3</v>
       </c>
@@ -1701,7 +1837,7 @@
         <v>Stimuli/3530.jpg</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
         <v>3</v>
       </c>
@@ -1716,7 +1852,7 @@
         <v>Stimuli/6212.jpg</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="1" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1867,7 @@
         <v>Stimuli/6415.jpg</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="1" t="s">
         <v>3</v>
       </c>
@@ -1746,7 +1882,7 @@
         <v>Stimuli/9250.jpg</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="1" t="s">
         <v>3</v>
       </c>
@@ -1761,7 +1897,7 @@
         <v>Stimuli/9253.jpg</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="1" t="s">
         <v>3</v>
       </c>
@@ -1776,7 +1912,7 @@
         <v>Stimuli/9373.jpg</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
@@ -1791,7 +1927,7 @@
         <v>Stimuli/9405.jpg</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="1" t="s">
         <v>3</v>
       </c>
@@ -1806,7 +1942,7 @@
         <v>Stimuli/9421.jpg</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="1" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +1957,7 @@
         <v>Stimuli/9425.jpg</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="1" t="s">
         <v>3</v>
       </c>
@@ -1836,7 +1972,7 @@
         <v>Stimuli/9433.jpg</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="1" t="s">
         <v>3</v>
       </c>
@@ -1851,7 +1987,7 @@
         <v>Stimuli/9490.jpg</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="1" t="s">
         <v>3</v>
       </c>
@@ -1866,7 +2002,7 @@
         <v>Stimuli/9520.jpg</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="1" t="s">
         <v>3</v>
       </c>
@@ -1881,7 +2017,7 @@
         <v>Stimuli/9560.jpg</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="1" t="s">
         <v>3</v>
       </c>
@@ -1896,7 +2032,7 @@
         <v>Stimuli/9599.jpg</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>